<commit_message>
Pandas makes data simple
</commit_message>
<xml_diff>
--- a/Final Product V.xlsx
+++ b/Final Product V.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\yonseiexchange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EE3795-0F17-426C-9D0D-4F608C525488}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF00873-8F67-4E8E-9F92-F5C905889BA2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="96" windowWidth="16332" windowHeight="10836" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -5061,8 +5061,8 @@
   </sheetPr>
   <dimension ref="A1:EK457"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="F170" sqref="F170"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>